<commit_message>
TDD also messages checked
</commit_message>
<xml_diff>
--- a/documentation/Design/TestCases.xlsx
+++ b/documentation/Design/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Peter/Development/Python/Fishing/V2/1_Preparation/fishing/documentation/Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF33F0F1-97F9-234D-A8B1-7391D200663A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15CCC14-3346-E247-9666-8C5F56300094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3700" yWindow="5440" windowWidth="28240" windowHeight="14140" activeTab="2" xr2:uid="{CB59B4E2-ABBB-9640-84E4-2E991D1E5FE4}"/>
+    <workbookView xWindow="6320" yWindow="6200" windowWidth="28240" windowHeight="14140" activeTab="2" xr2:uid="{CB59B4E2-ABBB-9640-84E4-2E991D1E5FE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Test cases" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="91">
   <si>
     <t>-</t>
   </si>
@@ -262,18 +262,6 @@
     <t>Post UserStatus</t>
   </si>
   <si>
-    <t>Expected HTTP</t>
-  </si>
-  <si>
-    <t>The user already exists.</t>
-  </si>
-  <si>
-    <t>The user is blocked. Please try again later.</t>
-  </si>
-  <si>
-    <t>The user is blacklisted.</t>
-  </si>
-  <si>
     <t>{"email": "dummy@sample.com", "password": "Right-Password01!"}</t>
   </si>
   <si>
@@ -284,6 +272,45 @@
   </si>
   <si>
     <t>{"email": "dummy@sample.com", "password": "Wrong-Password!", "new_password": "Right-New_Password1!",  "new_password_repeated": "Right-New_Password1!"}</t>
+  </si>
+  <si>
+    <t>Expected HTTP status</t>
+  </si>
+  <si>
+    <t>Expected response</t>
+  </si>
+  <si>
+    <t>{"detail": "The user already exists."}</t>
+  </si>
+  <si>
+    <t>{"detail": "The user is blacklisted."}</t>
+  </si>
+  <si>
+    <t>{"detail": "The user is blocked. Please try again later."}</t>
+  </si>
+  <si>
+    <t>{"detail": "The password is expired."}</t>
+  </si>
+  <si>
+    <t>{"type": "missing","loc": ["body", "password"],"msg": "Field required"}</t>
+  </si>
+  <si>
+    <t>{"type": "missing","loc": ["body", "new_password"],"msg": "Field required"}</t>
+  </si>
+  <si>
+    <t>{"type": "missing","loc": ["body", "email"],"msg": "Field required"}</t>
+  </si>
+  <si>
+    <t>{"detail": "Incorrect existing password. The user has been blocked. Please try again later."}</t>
+  </si>
+  <si>
+    <t>{"detail": "Incorrect existing password. Please try again."}</t>
+  </si>
+  <si>
+    <t>{"detail": "The password is not valid. The user has been blocked. Please try again later."}</t>
+  </si>
+  <si>
+    <t>{"detail": "The password is not valid. Please try again."}</t>
   </si>
 </sst>
 </file>
@@ -1469,8 +1496,8 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
+      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1484,14 +1511,14 @@
     <col min="7" max="7" width="29" style="36" customWidth="1"/>
     <col min="8" max="8" width="7" style="35" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.6640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29" style="36" customWidth="1"/>
     <col min="11" max="11" width="8.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -1517,10 +1544,10 @@
         <v>67</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>21</v>
+        <v>78</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>73</v>
@@ -1540,12 +1567,12 @@
       <c r="G2" s="1"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
-      <c r="J2" s="4"/>
+      <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="9"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>57</v>
       </c>
@@ -1573,8 +1600,8 @@
       <c r="I3" s="27">
         <v>422</v>
       </c>
-      <c r="J3" s="26" t="s">
-        <v>75</v>
+      <c r="J3" s="14" t="s">
+        <v>80</v>
       </c>
       <c r="K3" s="28" t="s">
         <v>66</v>
@@ -1607,7 +1634,7 @@
         <v>64</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H4" s="30">
         <v>0</v>
@@ -1615,8 +1642,8 @@
       <c r="I4" s="30">
         <v>401</v>
       </c>
-      <c r="J4" s="28" t="s">
-        <v>77</v>
+      <c r="J4" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="K4" s="28" t="s">
         <v>66</v>
@@ -1649,7 +1676,7 @@
         <v>64</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H5" s="30">
         <v>0</v>
@@ -1657,8 +1684,8 @@
       <c r="I5" s="30">
         <v>401</v>
       </c>
-      <c r="J5" s="28" t="s">
-        <v>77</v>
+      <c r="J5" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="K5" s="28" t="s">
         <v>66</v>
@@ -1699,8 +1726,8 @@
       <c r="I6" s="30">
         <v>401</v>
       </c>
-      <c r="J6" s="28" t="s">
-        <v>77</v>
+      <c r="J6" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="K6" s="28" t="s">
         <v>66</v>
@@ -1742,7 +1769,7 @@
         <v>422</v>
       </c>
       <c r="J7" s="31" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="K7" s="31" t="s">
         <v>66</v>
@@ -1775,7 +1802,7 @@
         <v>64</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H8" s="32">
         <v>0</v>
@@ -1784,7 +1811,7 @@
         <v>401</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="K8" s="31" t="s">
         <v>66</v>
@@ -1817,7 +1844,7 @@
         <v>64</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H9" s="32">
         <v>0</v>
@@ -1825,8 +1852,8 @@
       <c r="I9" s="32">
         <v>401</v>
       </c>
-      <c r="J9" s="31" t="s">
-        <v>76</v>
+      <c r="J9" s="25" t="s">
+        <v>82</v>
       </c>
       <c r="K9" s="31" t="s">
         <v>66</v>
@@ -1867,7 +1894,9 @@
       <c r="I10" s="32">
         <v>200</v>
       </c>
-      <c r="J10" s="31"/>
+      <c r="J10" s="31" t="s">
+        <v>69</v>
+      </c>
       <c r="K10" s="31">
         <v>10</v>
       </c>
@@ -1879,7 +1908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>58</v>
       </c>
@@ -1907,8 +1936,8 @@
       <c r="I11" s="27">
         <v>422</v>
       </c>
-      <c r="J11" s="26" t="s">
-        <v>75</v>
+      <c r="J11" s="14" t="s">
+        <v>80</v>
       </c>
       <c r="K11" s="28" t="s">
         <v>66</v>
@@ -1941,7 +1970,7 @@
         <v>64</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H12" s="30">
         <v>0</v>
@@ -1949,7 +1978,9 @@
       <c r="I12" s="30">
         <v>401</v>
       </c>
-      <c r="J12" s="28"/>
+      <c r="J12" s="14" t="s">
+        <v>83</v>
+      </c>
       <c r="K12" s="28" t="s">
         <v>66</v>
       </c>
@@ -1981,7 +2012,7 @@
         <v>64</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H13" s="30">
         <v>0</v>
@@ -1989,7 +2020,9 @@
       <c r="I13" s="30">
         <v>401</v>
       </c>
-      <c r="J13" s="28"/>
+      <c r="J13" s="14" t="s">
+        <v>83</v>
+      </c>
       <c r="K13" s="28" t="s">
         <v>66</v>
       </c>
@@ -2029,7 +2062,9 @@
       <c r="I14" s="30">
         <v>200</v>
       </c>
-      <c r="J14" s="28"/>
+      <c r="J14" s="14" t="s">
+        <v>69</v>
+      </c>
       <c r="K14" s="28">
         <v>10</v>
       </c>
@@ -2041,7 +2076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>61</v>
       </c>
@@ -2069,8 +2104,8 @@
       <c r="I15" s="32">
         <v>422</v>
       </c>
-      <c r="J15" s="31" t="s">
-        <v>75</v>
+      <c r="J15" s="22" t="s">
+        <v>80</v>
       </c>
       <c r="K15" s="31" t="s">
         <v>66</v>
@@ -2083,7 +2118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
         <v>61</v>
       </c>
@@ -2111,8 +2146,8 @@
       <c r="I16" s="32">
         <v>422</v>
       </c>
-      <c r="J16" s="31" t="s">
-        <v>75</v>
+      <c r="J16" s="22" t="s">
+        <v>80</v>
       </c>
       <c r="K16" s="31" t="s">
         <v>66</v>
@@ -2153,7 +2188,9 @@
       <c r="I17" s="32">
         <v>200</v>
       </c>
-      <c r="J17" s="31"/>
+      <c r="J17" s="22" t="s">
+        <v>69</v>
+      </c>
       <c r="K17" s="31">
         <v>10</v>
       </c>
@@ -2165,7 +2202,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>62</v>
       </c>
@@ -2193,7 +2230,9 @@
       <c r="I18" s="30">
         <v>422</v>
       </c>
-      <c r="J18" s="28"/>
+      <c r="J18" s="14" t="s">
+        <v>84</v>
+      </c>
       <c r="K18" s="28" t="s">
         <v>66</v>
       </c>
@@ -2205,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>62</v>
       </c>
@@ -2233,7 +2272,9 @@
       <c r="I19" s="30">
         <v>422</v>
       </c>
-      <c r="J19" s="28"/>
+      <c r="J19" s="14" t="s">
+        <v>85</v>
+      </c>
       <c r="K19" s="28" t="s">
         <v>66</v>
       </c>
@@ -2265,15 +2306,17 @@
         <v>64</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H20" s="30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I20" s="30">
         <v>401</v>
       </c>
-      <c r="J20" s="28"/>
+      <c r="J20" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="K20" s="28">
         <v>90</v>
       </c>
@@ -2305,15 +2348,17 @@
         <v>64</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H21" s="30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I21" s="30">
         <v>401</v>
       </c>
-      <c r="J21" s="28"/>
+      <c r="J21" s="18" t="s">
+        <v>88</v>
+      </c>
       <c r="K21" s="28" t="s">
         <v>66</v>
       </c>
@@ -2345,7 +2390,7 @@
         <v>65</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H22" s="30">
         <v>0</v>
@@ -2353,7 +2398,9 @@
       <c r="I22" s="30">
         <v>200</v>
       </c>
-      <c r="J22" s="28"/>
+      <c r="J22" s="18" t="s">
+        <v>69</v>
+      </c>
       <c r="K22" s="28">
         <v>20</v>
       </c>
@@ -2365,7 +2412,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="24" t="s">
         <v>42</v>
       </c>
@@ -2393,7 +2440,9 @@
       <c r="I23" s="32">
         <v>422</v>
       </c>
-      <c r="J23" s="31"/>
+      <c r="J23" s="22" t="s">
+        <v>84</v>
+      </c>
       <c r="K23" s="31" t="s">
         <v>66</v>
       </c>
@@ -2405,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
         <v>42</v>
       </c>
@@ -2428,12 +2477,14 @@
         <v>70</v>
       </c>
       <c r="H24" s="32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I24" s="32">
         <v>401</v>
       </c>
-      <c r="J24" s="31"/>
+      <c r="J24" s="22" t="s">
+        <v>89</v>
+      </c>
       <c r="K24" s="31">
         <v>90</v>
       </c>
@@ -2468,12 +2519,14 @@
         <v>70</v>
       </c>
       <c r="H25" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I25" s="32">
         <v>401</v>
       </c>
-      <c r="J25" s="31"/>
+      <c r="J25" s="22" t="s">
+        <v>90</v>
+      </c>
       <c r="K25" s="31" t="s">
         <v>66</v>
       </c>
@@ -2505,7 +2558,7 @@
         <v>65</v>
       </c>
       <c r="G26" s="22" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H26" s="32">
         <v>0</v>
@@ -2513,7 +2566,9 @@
       <c r="I26" s="32">
         <v>200</v>
       </c>
-      <c r="J26" s="31"/>
+      <c r="J26" s="22" t="s">
+        <v>69</v>
+      </c>
       <c r="K26" s="31" t="s">
         <v>66</v>
       </c>
@@ -2525,7 +2580,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
         <v>63</v>
       </c>
@@ -2553,7 +2608,9 @@
       <c r="I27" s="30">
         <v>422</v>
       </c>
-      <c r="J27" s="28"/>
+      <c r="J27" s="18" t="s">
+        <v>86</v>
+      </c>
       <c r="K27" s="28" t="s">
         <v>66</v>
       </c>
@@ -2593,7 +2650,9 @@
       <c r="I28" s="30">
         <v>200</v>
       </c>
-      <c r="J28" s="28"/>
+      <c r="J28" s="18" t="s">
+        <v>69</v>
+      </c>
       <c r="K28" s="28">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Add JWT token logic
</commit_message>
<xml_diff>
--- a/documentation/Design/TestCases.xlsx
+++ b/documentation/Design/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Peter/Development/Python/Fishing/V2/1_Preparation/fishing/documentation/Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C1F180-F488-7A4E-8F81-126952058280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B71655E-D8FC-254B-A99A-79DCD68A016B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="1100" windowWidth="22220" windowHeight="19300" activeTab="2" xr2:uid="{CB59B4E2-ABBB-9640-84E4-2E991D1E5FE4}"/>
   </bookViews>
@@ -205,9 +205,6 @@
     <t>login</t>
   </si>
   <si>
-    <t>set</t>
-  </si>
-  <si>
     <t>forgot</t>
   </si>
   <si>
@@ -226,9 +223,6 @@
     <t>Registration</t>
   </si>
   <si>
-    <t>Set password</t>
-  </si>
-  <si>
     <t>Forgot password</t>
   </si>
   <si>
@@ -317,6 +311,12 @@
   </si>
   <si>
     <t>The password is expired.</t>
+  </si>
+  <si>
+    <t>change</t>
+  </si>
+  <si>
+    <t>Change password</t>
   </si>
 </sst>
 </file>
@@ -1514,8 +1514,8 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1541,7 +1541,7 @@
         <v>51</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C1" s="38" t="s">
         <v>7</v>
@@ -1553,15 +1553,15 @@
         <v>12</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G1" s="39" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H1" s="38"/>
       <c r="I1" s="38"/>
       <c r="J1" s="39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K1" s="38"/>
       <c r="L1" s="38"/>
@@ -1577,26 +1577,26 @@
       <c r="E2" s="40"/>
       <c r="F2" s="40"/>
       <c r="G2" s="40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H2" s="40" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I2" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="K2" s="40" t="s">
         <v>79</v>
-      </c>
-      <c r="K2" s="40" t="s">
-        <v>81</v>
       </c>
       <c r="L2" s="40"/>
       <c r="M2" s="40"/>
     </row>
     <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="26">
         <v>1</v>
@@ -1608,7 +1608,7 @@
         <v>54</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F3" s="27">
         <v>0</v>
@@ -1617,16 +1617,16 @@
         <v>422</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J3" s="26">
         <v>99</v>
       </c>
       <c r="K3" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L3" s="15" t="str">
         <f>_xlfn.IFNA(VLOOKUP(H3,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="28">
         <v>2</v>
@@ -1650,7 +1650,7 @@
         <v>54</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F4" s="30">
         <v>0</v>
@@ -1659,16 +1659,16 @@
         <v>401</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J4" s="28">
         <v>99</v>
       </c>
       <c r="K4" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L4" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(H4,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -1680,19 +1680,19 @@
     </row>
     <row r="5" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="28">
         <v>3</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F5" s="30">
         <v>0</v>
@@ -1701,16 +1701,16 @@
         <v>401</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J5" s="28">
         <v>99</v>
       </c>
       <c r="K5" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L5" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(H5,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -1722,19 +1722,19 @@
     </row>
     <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="28">
         <v>4</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F6" s="30">
         <v>0</v>
@@ -1743,16 +1743,16 @@
         <v>401</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J6" s="28">
         <v>99</v>
       </c>
       <c r="K6" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L6" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(H6,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="31">
         <v>5</v>
@@ -1776,7 +1776,7 @@
         <v>54</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F7" s="32">
         <v>0</v>
@@ -1785,16 +1785,16 @@
         <v>422</v>
       </c>
       <c r="H7" s="41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J7" s="31">
         <v>90</v>
       </c>
       <c r="K7" s="31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L7" s="23" t="str">
         <f>_xlfn.IFNA(VLOOKUP(K7,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -1806,7 +1806,7 @@
     </row>
     <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="31">
         <v>6</v>
@@ -1818,7 +1818,7 @@
         <v>54</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F8" s="32">
         <v>0</v>
@@ -1827,16 +1827,16 @@
         <v>401</v>
       </c>
       <c r="H8" s="41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I8" s="31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J8" s="31">
         <v>90</v>
       </c>
       <c r="K8" s="31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L8" s="23" t="str">
         <f>_xlfn.IFNA(VLOOKUP(K8,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -1848,19 +1848,19 @@
     </row>
     <row r="9" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="31">
         <v>7</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>55</v>
+      <c r="C9" s="17" t="s">
+        <v>91</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F9" s="32">
         <v>0</v>
@@ -1869,16 +1869,16 @@
         <v>401</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J9" s="31">
         <v>90</v>
       </c>
       <c r="K9" s="31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L9" s="23" t="str">
         <f>_xlfn.IFNA(VLOOKUP(K9,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -1890,19 +1890,19 @@
     </row>
     <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="31">
         <v>8</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>39</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F10" s="32">
         <v>0</v>
@@ -1911,7 +1911,7 @@
         <v>200</v>
       </c>
       <c r="H10" s="41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I10" s="31"/>
       <c r="J10" s="31">
@@ -1930,7 +1930,7 @@
     </row>
     <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="28">
         <v>9</v>
@@ -1942,7 +1942,7 @@
         <v>54</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F11" s="30">
         <v>0</v>
@@ -1951,16 +1951,16 @@
         <v>422</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J11" s="28">
         <v>80</v>
       </c>
       <c r="K11" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L11" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(K11,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -1972,7 +1972,7 @@
     </row>
     <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="28">
         <v>10</v>
@@ -1984,7 +1984,7 @@
         <v>54</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F12" s="30">
         <v>0</v>
@@ -1993,16 +1993,16 @@
         <v>401</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J12" s="28">
         <v>80</v>
       </c>
       <c r="K12" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L12" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(K12,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -2014,19 +2014,19 @@
     </row>
     <row r="13" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="28">
         <v>11</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F13" s="30">
         <v>0</v>
@@ -2035,16 +2035,16 @@
         <v>401</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J13" s="28">
         <v>80</v>
       </c>
       <c r="K13" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L13" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(K13,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -2056,19 +2056,19 @@
     </row>
     <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="28">
         <v>12</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F14" s="30">
         <v>0</v>
@@ -2077,7 +2077,7 @@
         <v>200</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I14" s="14"/>
       <c r="J14" s="28">
@@ -2096,7 +2096,7 @@
     </row>
     <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="31">
         <v>13</v>
@@ -2108,7 +2108,7 @@
         <v>54</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F15" s="32">
         <v>0</v>
@@ -2117,16 +2117,16 @@
         <v>422</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J15" s="31">
         <v>10</v>
       </c>
       <c r="K15" s="31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L15" s="23" t="str">
         <f>_xlfn.IFNA(VLOOKUP(K15,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -2138,7 +2138,7 @@
     </row>
     <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="31">
         <v>14</v>
@@ -2150,7 +2150,7 @@
         <v>54</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F16" s="32">
         <v>0</v>
@@ -2159,16 +2159,16 @@
         <v>422</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I16" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J16" s="31">
         <v>20</v>
       </c>
       <c r="K16" s="31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L16" s="23" t="str">
         <f>_xlfn.IFNA(VLOOKUP(K16,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -2180,7 +2180,7 @@
     </row>
     <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="21">
         <v>15</v>
@@ -2192,7 +2192,7 @@
         <v>54</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F17" s="32">
         <v>0</v>
@@ -2201,11 +2201,11 @@
         <v>200</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I17" s="22"/>
       <c r="J17" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K17" s="31">
         <v>10</v>
@@ -2220,19 +2220,19 @@
     </row>
     <row r="18" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="B18" s="28">
         <v>16</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F18" s="30">
         <v>0</v>
@@ -2241,14 +2241,14 @@
         <v>422</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I18" s="14"/>
       <c r="J18" s="28">
         <v>20</v>
       </c>
       <c r="K18" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L18" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(K18,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -2260,19 +2260,19 @@
     </row>
     <row r="19" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="B19" s="28">
         <v>17</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F19" s="30">
         <v>0</v>
@@ -2281,14 +2281,14 @@
         <v>422</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I19" s="14"/>
       <c r="J19" s="28">
         <v>10</v>
       </c>
       <c r="K19" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L19" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(K19,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -2300,19 +2300,19 @@
     </row>
     <row r="20" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="B20" s="28">
         <v>18</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F20" s="30">
         <v>4</v>
@@ -2321,10 +2321,10 @@
         <v>401</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J20" s="28">
         <v>10</v>
@@ -2342,19 +2342,19 @@
     </row>
     <row r="21" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="B21" s="28">
         <v>19</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F21" s="30">
         <v>3</v>
@@ -2363,16 +2363,16 @@
         <v>401</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J21" s="28">
         <v>10</v>
       </c>
       <c r="K21" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L21" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(K21,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -2384,19 +2384,19 @@
     </row>
     <row r="22" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="B22" s="28">
         <v>20</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F22" s="30">
         <v>0</v>
@@ -2405,7 +2405,7 @@
         <v>200</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I22" s="18"/>
       <c r="J22" s="28">
@@ -2436,7 +2436,7 @@
         <v>54</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F23" s="32">
         <v>0</v>
@@ -2445,14 +2445,14 @@
         <v>422</v>
       </c>
       <c r="H23" s="22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I23" s="22"/>
       <c r="J23" s="31">
         <v>10</v>
       </c>
       <c r="K23" s="31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L23" s="23" t="str">
         <f>_xlfn.IFNA(VLOOKUP(K23,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -2476,7 +2476,7 @@
         <v>54</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F24" s="32">
         <v>4</v>
@@ -2485,10 +2485,10 @@
         <v>401</v>
       </c>
       <c r="H24" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J24" s="31">
         <v>20</v>
@@ -2518,7 +2518,7 @@
         <v>54</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F25" s="32">
         <v>3</v>
@@ -2527,16 +2527,16 @@
         <v>401</v>
       </c>
       <c r="H25" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J25" s="31">
         <v>20</v>
       </c>
       <c r="K25" s="31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L25" s="23" t="str">
         <f>_xlfn.IFNA(VLOOKUP(K25,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -2560,7 +2560,7 @@
         <v>54</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F26" s="32">
         <v>0</v>
@@ -2569,14 +2569,14 @@
         <v>200</v>
       </c>
       <c r="H26" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I26" s="22"/>
       <c r="J26" s="31">
         <v>20</v>
       </c>
       <c r="K26" s="31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L26" s="23" t="str">
         <f>_xlfn.IFNA(VLOOKUP(K26,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -2588,19 +2588,19 @@
     </row>
     <row r="27" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B27" s="28">
         <v>25</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F27" s="30">
         <v>0</v>
@@ -2609,14 +2609,14 @@
         <v>422</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I27" s="18"/>
       <c r="J27" s="28">
         <v>10</v>
       </c>
       <c r="K27" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L27" s="19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(K27,State!$A$3:$B$8,2,FALSE),"")</f>
@@ -2628,19 +2628,19 @@
     </row>
     <row r="28" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B28" s="28">
         <v>26</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F28" s="30">
         <v>0</v>
@@ -2649,7 +2649,7 @@
         <v>200</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I28" s="18"/>
       <c r="J28" s="28">

</xml_diff>

<commit_message>
Authentication - Activate endpoint added
</commit_message>
<xml_diff>
--- a/documentation/Design/TestCases.xlsx
+++ b/documentation/Design/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Peter/Development/Python/Fishing/V2/1_Preparation/fishing/documentation/Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863A521F-964C-3C47-B090-B0176890ABF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1FC815-C5C0-8E4E-BC54-AFDF91DCDCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="1100" windowWidth="22220" windowHeight="19300" activeTab="2" xr2:uid="{CB59B4E2-ABBB-9640-84E4-2E991D1E5FE4}"/>
   </bookViews>
@@ -1508,8 +1508,8 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2309,7 +2309,7 @@
         <v>71</v>
       </c>
       <c r="F20" s="30">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G20" s="30">
         <v>401</v>
@@ -2473,7 +2473,7 @@
         <v>66</v>
       </c>
       <c r="F24" s="32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G24" s="32">
         <v>401</v>

</xml_diff>